<commit_message>
number of authors and inst
</commit_message>
<xml_diff>
--- a/php/src/planilha.xlsx
+++ b/php/src/planilha.xlsx
@@ -52,7 +52,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:34">
       <c r="A1" s="0" t="inlineStr">
         <is>
           <t>ID</t>
@@ -70,12 +70,157 @@
       </c>
       <c r="D1" s="0" t="inlineStr">
         <is>
-          <t>Author1</t>
+          <t>Author 1</t>
         </is>
       </c>
       <c r="E1" s="0" t="inlineStr">
         <is>
+          <t>Author 2</t>
+        </is>
+      </c>
+      <c r="F1" s="0" t="inlineStr">
+        <is>
+          <t>Author 3</t>
+        </is>
+      </c>
+      <c r="G1" s="0" t="inlineStr">
+        <is>
+          <t>Author 4</t>
+        </is>
+      </c>
+      <c r="H1" s="0" t="inlineStr">
+        <is>
+          <t>Author 5</t>
+        </is>
+      </c>
+      <c r="I1" s="0" t="inlineStr">
+        <is>
+          <t>Author 6</t>
+        </is>
+      </c>
+      <c r="J1" s="0" t="inlineStr">
+        <is>
+          <t>Author 7</t>
+        </is>
+      </c>
+      <c r="K1" s="0" t="inlineStr">
+        <is>
+          <t>Author 8</t>
+        </is>
+      </c>
+      <c r="L1" s="0" t="inlineStr">
+        <is>
+          <t>Author 9</t>
+        </is>
+      </c>
+      <c r="M1" s="0" t="inlineStr">
+        <is>
+          <t>Author 10</t>
+        </is>
+      </c>
+      <c r="N1" s="0" t="inlineStr">
+        <is>
+          <t>Author 1</t>
+        </is>
+      </c>
+      <c r="O1" s="0" t="inlineStr">
+        <is>
+          <t>Author 12</t>
+        </is>
+      </c>
+      <c r="P1" s="0" t="inlineStr">
+        <is>
+          <t>Author 13</t>
+        </is>
+      </c>
+      <c r="Q1" s="0" t="inlineStr">
+        <is>
+          <t>Author 14</t>
+        </is>
+      </c>
+      <c r="R1" s="0" t="inlineStr">
+        <is>
+          <t>Author 15</t>
+        </is>
+      </c>
+      <c r="S1" s="0" t="inlineStr">
+        <is>
           <t>Institution 1</t>
+        </is>
+      </c>
+      <c r="T1" s="0" t="inlineStr">
+        <is>
+          <t>Institution 2</t>
+        </is>
+      </c>
+      <c r="U1" s="0" t="inlineStr">
+        <is>
+          <t>Institution 3</t>
+        </is>
+      </c>
+      <c r="V1" s="0" t="inlineStr">
+        <is>
+          <t>Institution 4</t>
+        </is>
+      </c>
+      <c r="W1" s="0" t="inlineStr">
+        <is>
+          <t>Institution 5</t>
+        </is>
+      </c>
+      <c r="X1" s="0" t="inlineStr">
+        <is>
+          <t>Institution 6</t>
+        </is>
+      </c>
+      <c r="Y1" s="0" t="inlineStr">
+        <is>
+          <t>Institution 7</t>
+        </is>
+      </c>
+      <c r="Z1" s="0" t="inlineStr">
+        <is>
+          <t>Institution 8</t>
+        </is>
+      </c>
+      <c r="AA1" s="0" t="inlineStr">
+        <is>
+          <t>Institution 9</t>
+        </is>
+      </c>
+      <c r="AB1" s="0" t="inlineStr">
+        <is>
+          <t>Institution 10</t>
+        </is>
+      </c>
+      <c r="AC1" s="0" t="inlineStr">
+        <is>
+          <t>Institution 11</t>
+        </is>
+      </c>
+      <c r="AD1" s="0" t="inlineStr">
+        <is>
+          <t>Institution 12</t>
+        </is>
+      </c>
+      <c r="AE1" s="0" t="inlineStr">
+        <is>
+          <t>Institution 13</t>
+        </is>
+      </c>
+      <c r="AF1" s="0" t="inlineStr">
+        <is>
+          <t>Institution 14</t>
+        </is>
+      </c>
+      <c r="AG1" s="0" t="inlineStr">
+        <is>
+          <t>Institution 15</t>
+        </is>
+      </c>
+      <c r="AH1" s="0" t="inlineStr">
+        <is>
+          <t>Institution 16</t>
         </is>
       </c>
     </row>

</xml_diff>